<commit_message>
oke, import excel bahasa, faq, keterampilan, mata uang
</commit_message>
<xml_diff>
--- a/public/assets/excel/file-format-import-mata-uang.xlsx
+++ b/public/assets/excel/file-format-import-mata-uang.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>KODE</t>
+    <t>NEGARA</t>
   </si>
   <si>
-    <t>NEGARA</t>
+    <t>KODE ( Unik =&gt; Maks 4 karakter )</t>
   </si>
 </sst>
 </file>
@@ -336,22 +336,22 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>